<commit_message>
refactor code. Empty string token bug?
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Progs\git\kl_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4421D76D-E985-4046-88A9-D86E9FDA43A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D00AB93-4049-474C-8423-138C93ACF68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F9E28195-B5B3-4303-86E3-79F783E79393}"/>
   </bookViews>
@@ -288,13 +288,19 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -477,7 +483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -567,6 +573,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -886,7 +895,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,8 +1257,8 @@
         <v>73</v>
       </c>
       <c r="C24" s="15"/>
-      <c r="D24" s="4">
-        <v>400</v>
+      <c r="D24" s="31">
+        <v>401</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>74</v>

</xml_diff>